<commit_message>
fix db queries and tasks
</commit_message>
<xml_diff>
--- a/app/admin/Menu.xlsx
+++ b/app/admin/Menu.xlsx
@@ -277,31 +277,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -322,294 +322,297 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="77.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="48.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="47.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="49.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="77.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="2"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="2"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="3" t="n">
         <v>182.99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="4" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="3" t="n">
         <v>215.36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="4" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="3" t="n">
         <v>265.57</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="3" t="n">
         <v>166.47</v>
       </c>
+      <c r="G7" s="0" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="3" t="n">
         <v>168.25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="3" t="n">
         <v>132.88</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="2"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="2"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="4" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="3" t="n">
         <v>2700.79</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="4" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="3" t="n">
         <v>3100.33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="4" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="3" t="n">
         <v>1850.42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="2"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="3" t="n">
         <v>420.78</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="3" t="n">
         <v>440.11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="3" t="n">
         <v>520.08</v>
       </c>
     </row>

</xml_diff>